<commit_message>
Add column to validParameters table
The 'UnitRegexp' column is used to match multiple ways of writing the
specific unit.
</commit_message>
<xml_diff>
--- a/+DataKit/ressources/validParameters.xlsx
+++ b/+DataKit/ressources/validParameters.xlsx
@@ -8,32 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/+DataKit/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2BF96C-2160-E343-AE2E-4851CF0AA00B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E32D11-1A83-FF4E-A62C-77BB58D90DB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{87387DFF-398A-9541-805A-AB9ACB3A02A8}"/>
+    <workbookView xWindow="2800" yWindow="1580" windowWidth="28800" windowHeight="12740" xr2:uid="{87387DFF-398A-9541-805A-AB9ACB3A02A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
   <si>
     <t>ParameterId</t>
   </si>
@@ -321,6 +313,12 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>UnitSynonyms</t>
+  </si>
+  <si>
+    <t>µmol L⁻¹</t>
   </si>
 </sst>
 </file>
@@ -686,10 +684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35489B87-C427-6749-AB7C-AF37172BFD7E}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <pane ySplit="4" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,7 +698,7 @@
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,13 +718,16 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -747,11 +749,14 @@
       <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -770,11 +775,11 @@
       <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>26498</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -793,11 +798,11 @@
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>735</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -816,11 +821,11 @@
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>186962</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -839,11 +844,11 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>18829</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -862,11 +867,11 @@
       <c r="F9" t="s">
         <v>18</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>26499</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -885,11 +890,11 @@
       <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -905,14 +910,14 @@
       <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>29</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -928,14 +933,14 @@
       <c r="F12" t="s">
         <v>18</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>30</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -954,11 +959,14 @@
       <c r="F13" t="s">
         <v>32</v>
       </c>
-      <c r="H13">
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13">
         <v>757</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -977,11 +985,11 @@
       <c r="F14" t="s">
         <v>32</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>756</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1000,11 +1008,11 @@
       <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>758</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1023,11 +1031,11 @@
       <c r="F16" t="s">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>755</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1046,11 +1054,11 @@
       <c r="F17" t="s">
         <v>32</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1067,7 +1075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1086,11 +1094,11 @@
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>754</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1107,7 +1115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1124,7 +1132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1140,11 +1148,11 @@
       <c r="F22" t="s">
         <v>60</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>716</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1161,7 +1169,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1195,7 +1203,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1212,7 +1220,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1229,7 +1237,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1246,7 +1254,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1263,7 +1271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1280,7 +1288,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1297,7 +1305,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1316,11 +1324,11 @@
       <c r="F32" t="s">
         <v>89</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1339,11 +1347,11 @@
       <c r="F33" t="s">
         <v>32</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>161330</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1362,7 +1370,7 @@
       <c r="F34" t="s">
         <v>89</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Readd column to validParameters table
The 'UnitRegexp' column is used to match multiple ways of writing the
specific unit.
</commit_message>
<xml_diff>
--- a/+DataKit/ressources/validParameters.xlsx
+++ b/+DataKit/ressources/validParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/+DataKit/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E32D11-1A83-FF4E-A62C-77BB58D90DB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A66E95-405B-2542-B6EB-85C575981D0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1580" windowWidth="28800" windowHeight="12740" xr2:uid="{87387DFF-398A-9541-805A-AB9ACB3A02A8}"/>
+    <workbookView xWindow="2780" yWindow="1060" windowWidth="28800" windowHeight="12740" xr2:uid="{87387DFF-398A-9541-805A-AB9ACB3A02A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="108">
   <si>
     <t>ParameterId</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Salinity</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>lux</t>
   </si>
   <si>
@@ -315,10 +312,43 @@
     <t>A2</t>
   </si>
   <si>
-    <t>UnitSynonyms</t>
-  </si>
-  <si>
-    <t>µmol L⁻¹</t>
+    <t>UnitRegexp</t>
+  </si>
+  <si>
+    <t>(µ|u)mol(\sL(⁻¹|-1)|/L)</t>
+  </si>
+  <si>
+    <t>mmol(\sL(⁻¹|-1)|/L)</t>
+  </si>
+  <si>
+    <t>m(\ss(⁻¹|-1)|/s)</t>
+  </si>
+  <si>
+    <t>kg(\sm(⁻³|-3)|(/m|/m³)</t>
+  </si>
+  <si>
+    <t>mS(\scm(⁻¹|-1)|/cm)</t>
+  </si>
+  <si>
+    <t>d(|eci)b(|ar)</t>
+  </si>
+  <si>
+    <t>(°|deg\s?)C</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>(PSU|psu)</t>
+  </si>
+  <si>
+    <t>(C|c)ounts</t>
+  </si>
+  <si>
+    <t>(L|l)ux</t>
+  </si>
+  <si>
+    <t>(NTU|ntu)</t>
   </si>
 </sst>
 </file>
@@ -687,8 +717,8 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,6 +726,7 @@
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -718,7 +749,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
         <v>28</v>
@@ -775,6 +806,9 @@
       <c r="F5" t="s">
         <v>18</v>
       </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
       <c r="I5">
         <v>26498</v>
       </c>
@@ -798,6 +832,9 @@
       <c r="F6" t="s">
         <v>18</v>
       </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
       <c r="I6">
         <v>735</v>
       </c>
@@ -821,6 +858,9 @@
       <c r="F7" t="s">
         <v>18</v>
       </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
       <c r="I7">
         <v>186962</v>
       </c>
@@ -844,6 +884,9 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
       <c r="I8">
         <v>18829</v>
       </c>
@@ -867,6 +910,9 @@
       <c r="F9" t="s">
         <v>18</v>
       </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
       <c r="I9">
         <v>26499</v>
       </c>
@@ -890,6 +936,9 @@
       <c r="F10" t="s">
         <v>18</v>
       </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
       <c r="I10">
         <v>70</v>
       </c>
@@ -908,6 +957,9 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
         <v>20</v>
       </c>
       <c r="H11" t="s">
@@ -933,6 +985,9 @@
       <c r="F12" t="s">
         <v>18</v>
       </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
       <c r="H12" t="s">
         <v>30</v>
       </c>
@@ -960,7 +1015,7 @@
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13">
         <v>757</v>
@@ -985,6 +1040,9 @@
       <c r="F14" t="s">
         <v>32</v>
       </c>
+      <c r="G14" t="s">
+        <v>96</v>
+      </c>
       <c r="I14">
         <v>756</v>
       </c>
@@ -1008,6 +1066,9 @@
       <c r="F15" t="s">
         <v>32</v>
       </c>
+      <c r="G15" t="s">
+        <v>96</v>
+      </c>
       <c r="I15">
         <v>758</v>
       </c>
@@ -1031,6 +1092,9 @@
       <c r="F16" t="s">
         <v>32</v>
       </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
       <c r="I16">
         <v>755</v>
       </c>
@@ -1054,6 +1118,9 @@
       <c r="F17" t="s">
         <v>32</v>
       </c>
+      <c r="G17" t="s">
+        <v>96</v>
+      </c>
       <c r="I17">
         <v>52</v>
       </c>
@@ -1074,6 +1141,9 @@
       <c r="F18" t="s">
         <v>48</v>
       </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1094,6 +1164,9 @@
       <c r="F19" t="s">
         <v>32</v>
       </c>
+      <c r="G19" t="s">
+        <v>96</v>
+      </c>
       <c r="I19">
         <v>754</v>
       </c>
@@ -1114,6 +1187,9 @@
       <c r="F20" t="s">
         <v>54</v>
       </c>
+      <c r="G20" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1131,6 +1207,9 @@
       <c r="F21" t="s">
         <v>57</v>
       </c>
+      <c r="G21" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -1146,7 +1225,10 @@
         <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>103</v>
+      </c>
+      <c r="G22" t="s">
+        <v>104</v>
       </c>
       <c r="I22">
         <v>716</v>
@@ -1157,16 +1239,19 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1174,16 +1259,19 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G24" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1191,16 +1279,19 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
         <v>66</v>
       </c>
-      <c r="F25" t="s">
-        <v>67</v>
+      <c r="G25" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1208,16 +1299,19 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>69</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>70</v>
       </c>
-      <c r="F26" t="s">
-        <v>71</v>
+      <c r="G26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1225,16 +1319,19 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" t="s">
         <v>73</v>
       </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" t="s">
-        <v>74</v>
+      <c r="G27" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1242,16 +1339,19 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
         <v>75</v>
       </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>76</v>
       </c>
-      <c r="F28" t="s">
-        <v>77</v>
+      <c r="G28" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1259,16 +1359,19 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>79</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>80</v>
       </c>
-      <c r="F29" t="s">
-        <v>81</v>
+      <c r="G29" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1276,16 +1379,19 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G30" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1293,16 +1399,19 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G31" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1310,19 +1419,22 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
         <v>87</v>
       </c>
-      <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
         <v>88</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>89</v>
+      <c r="G32" t="s">
+        <v>97</v>
       </c>
       <c r="I32">
         <v>54</v>
@@ -1333,19 +1445,22 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
         <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" t="s">
-        <v>91</v>
       </c>
       <c r="E33" t="s">
         <v>7</v>
       </c>
       <c r="F33" t="s">
         <v>32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>97</v>
       </c>
       <c r="I33">
         <v>161330</v>
@@ -1356,19 +1471,22 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
         <v>92</v>
       </c>
-      <c r="C34" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" t="s">
-        <v>93</v>
-      </c>
       <c r="E34" t="s">
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="G34" t="s">
+        <v>97</v>
       </c>
       <c r="I34">
         <v>50</v>

</xml_diff>